<commit_message>
excel and angular routing
</commit_message>
<xml_diff>
--- a/ExcelDemo/playerWorkbook.xlsx
+++ b/ExcelDemo/playerWorkbook.xlsx
@@ -12,20 +12,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>League</t>
+  </si>
   <si>
     <t>Adam</t>
   </si>
   <si>
+    <t>Blues</t>
+  </si>
+  <si>
+    <t>Premier</t>
+  </si>
+  <si>
     <t>Bob</t>
   </si>
   <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>League 1</t>
+  </si>
+  <si>
     <t>Charlie</t>
   </si>
   <si>
     <t>Dean</t>
   </si>
   <si>
+    <t>Reds</t>
+  </si>
+  <si>
     <t>Elias</t>
   </si>
   <si>
@@ -33,6 +66,9 @@
   </si>
   <si>
     <t>Grant</t>
+  </si>
+  <si>
+    <t>United</t>
   </si>
   <si>
     <t>Harry</t>
@@ -80,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -90,40 +126,180 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B6" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="B7" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="B8" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>